<commit_message>
Update the sample ooxml files to the latest versions from http://openxmldeveloper.org/articles/SampleDocsAugust2007.aspx (previous samples were from a beta)
git-svn-id: https://svn.apache.org/repos/asf/poi/trunk@606920 13f79535-47bb-0310-9956-ffa450edef68
</commit_message>
<xml_diff>
--- a/src/testcases/org/apache/poi/hssf/data/sample.xlsx
+++ b/src/testcases/org/apache/poi/hssf/data/sample.xlsx
@@ -1,63 +1,63 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.microsoft.com/office/excel/2006/2" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
-  <workbookPr autoCompressPictures="0"/>
-  <calcPr calcId="122211" fullCalcOnLoad="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="15480" windowHeight="10560"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="20055" windowHeight="12240"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <webPublishing codePage="1252"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.microsoft.com/office/excel/2006/2" xml:space="preserve" count="10" uniqueCount="10">
-  <sstItem>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
     <t>Lorem</t>
-  </sstItem>
-  <sstItem>
+  </si>
+  <si>
     <t>ipsum</t>
-  </sstItem>
-  <sstItem>
+  </si>
+  <si>
     <t>dolor</t>
-  </sstItem>
-  <sstItem>
+  </si>
+  <si>
     <t>sit</t>
-  </sstItem>
-  <sstItem>
+  </si>
+  <si>
     <t>amet</t>
-  </sstItem>
-  <sstItem>
+  </si>
+  <si>
     <t>consectetuer</t>
-  </sstItem>
-  <sstItem>
+  </si>
+  <si>
     <t>adipiscing</t>
-  </sstItem>
-  <sstItem>
+  </si>
+  <si>
     <t>elit</t>
-  </sstItem>
-  <sstItem>
+  </si>
+  <si>
     <t>Nunc</t>
-  </sstItem>
-  <sstItem>
+  </si>
+  <si>
     <t>at</t>
-  </sstItem>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.microsoft.com/office/excel/2006/2" xml:space="preserve">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -82,65 +82,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
-  <colors>
-    <themeColors>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFAF3E8"/>
-      <rgbColor rgb="FF1F497D"/>
-      <rgbColor rgb="FF5C83B4"/>
-      <rgbColor rgb="FFC0504D"/>
-      <rgbColor rgb="FF9DBB61"/>
-      <rgbColor rgb="FF8066A0"/>
-      <rgbColor rgb="FF4BACC6"/>
-      <rgbColor rgb="FFF59D56"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF800080"/>
-    </themeColors>
-  </colors>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/3/main" name="Custom Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office Colors">
+    <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="FAF3E8"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5C83B4"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9DBB61"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8066A0"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
         <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F59D56"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
         <a:srgbClr val="0000FF"/>
@@ -149,48 +133,99 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office Fonts">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office Effects">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="100000"/>
-            <a:shade val="100000"/>
-            <a:satMod val="100000"/>
-          </a:schemeClr>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="65000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="133000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="15000">
-              <a:schemeClr val="phClr">
                 <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="140000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="10000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="135000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -200,43 +235,43 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="75000"/>
-                <a:satMod val="160000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="62000">
-              <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="125000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="140000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="12700">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -246,123 +281,91 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="50800" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="43137"/>
+                <a:alpha val="38000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="50800" dist="38100" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="61176"/>
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
           <a:scene3d>
-            <a:camera prst="orthographicFront" fov="0">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="contrasting" dir="t">
-              <a:rot lat="0" lon="0" rev="16500000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d contourW="12700" prstMaterial="powder">
-            <a:bevelT h="50800"/>
-            <a:contourClr>
-              <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="100000"/>
-              </a:schemeClr>
-            </a:contourClr>
-          </a:sp3d>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:reflection blurRad="12700" stA="25000" endPos="28000" dist="38100" dir="5400000" sy="-100000" rotWithShape="0"/>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront" fov="0">
+            <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
             <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="139700" h="38100"/>
-            <a:contourClr>
-              <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="100000"/>
-              </a:schemeClr>
-            </a:contourClr>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="100000"/>
-            <a:shade val="100000"/>
-            <a:satMod val="100000"/>
-          </a:schemeClr>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="50000"/>
-                <a:satMod val="145000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="70000"/>
-                <a:satMod val="145000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="85000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="155000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="50000"/>
-                <a:satMod val="145000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="30000">
-              <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="65000"/>
-                <a:satMod val="155000"/>
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="60000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="170000"/>
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -373,19 +376,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.microsoft.com/office/excel/2006/2" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:2" customFormat="1">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -393,7 +391,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:2" customFormat="1">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -401,7 +399,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="3" spans="1:2" customFormat="1">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -409,7 +407,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="4" spans="1:2" customFormat="1">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -417,7 +415,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="5" spans="1:2" customFormat="1">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -425,7 +423,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="6" spans="1:2" customFormat="1">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -433,7 +431,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="7" spans="1:2" customFormat="1">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -441,7 +439,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="8" spans="1:2" customFormat="1">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -449,7 +447,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="9" spans="1:2" customFormat="1">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -457,7 +455,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="10" spans="1:2" customFormat="1">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -467,43 +465,33 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection objects="0" scenarios="0"/>
-  <printOptions/>
-  <pageMargins left="0.35" right="0.35" top="0.75" bottom="0.75" header="0.25" footer="0.25"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.microsoft.com/office/excel/2006/2" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
-  <sheetProtection objects="0" scenarios="0"/>
-  <printOptions/>
-  <pageMargins left="0.35" right="0.35" top="0.75" bottom="0.75" header="0.25" footer="0.25"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.microsoft.com/office/excel/2006/2" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
-  <sheetProtection objects="0" scenarios="0"/>
-  <printOptions/>
-  <pageMargins left="0.35" right="0.35" top="0.75" bottom="0.75" header="0.25" footer="0.25"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
merged TRUNK changes r608809 into REL_3_0_2_BETA2
git-svn-id: https://svn.apache.org/repos/asf/poi/tags/REL_3_0_2_BETA2@608846 13f79535-47bb-0310-9956-ffa450edef68
</commit_message>
<xml_diff>
--- a/src/testcases/org/apache/poi/hssf/data/sample.xlsx
+++ b/src/testcases/org/apache/poi/hssf/data/sample.xlsx
@@ -1,63 +1,63 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.microsoft.com/office/excel/2006/2" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
-  <workbookPr autoCompressPictures="0"/>
-  <calcPr calcId="122211" fullCalcOnLoad="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="15480" windowHeight="10560"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="20055" windowHeight="12240"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <webPublishing codePage="1252"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.microsoft.com/office/excel/2006/2" xml:space="preserve" count="10" uniqueCount="10">
-  <sstItem>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
     <t>Lorem</t>
-  </sstItem>
-  <sstItem>
+  </si>
+  <si>
     <t>ipsum</t>
-  </sstItem>
-  <sstItem>
+  </si>
+  <si>
     <t>dolor</t>
-  </sstItem>
-  <sstItem>
+  </si>
+  <si>
     <t>sit</t>
-  </sstItem>
-  <sstItem>
+  </si>
+  <si>
     <t>amet</t>
-  </sstItem>
-  <sstItem>
+  </si>
+  <si>
     <t>consectetuer</t>
-  </sstItem>
-  <sstItem>
+  </si>
+  <si>
     <t>adipiscing</t>
-  </sstItem>
-  <sstItem>
+  </si>
+  <si>
     <t>elit</t>
-  </sstItem>
-  <sstItem>
+  </si>
+  <si>
     <t>Nunc</t>
-  </sstItem>
-  <sstItem>
+  </si>
+  <si>
     <t>at</t>
-  </sstItem>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.microsoft.com/office/excel/2006/2" xml:space="preserve">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -82,65 +82,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
-  <colors>
-    <themeColors>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFAF3E8"/>
-      <rgbColor rgb="FF1F497D"/>
-      <rgbColor rgb="FF5C83B4"/>
-      <rgbColor rgb="FFC0504D"/>
-      <rgbColor rgb="FF9DBB61"/>
-      <rgbColor rgb="FF8066A0"/>
-      <rgbColor rgb="FF4BACC6"/>
-      <rgbColor rgb="FFF59D56"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF800080"/>
-    </themeColors>
-  </colors>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/3/main" name="Custom Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office Colors">
+    <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="FAF3E8"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5C83B4"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9DBB61"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8066A0"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
         <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F59D56"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
         <a:srgbClr val="0000FF"/>
@@ -149,48 +133,99 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office Fonts">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office Effects">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="100000"/>
-            <a:shade val="100000"/>
-            <a:satMod val="100000"/>
-          </a:schemeClr>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="65000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="133000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="15000">
-              <a:schemeClr val="phClr">
                 <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="140000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="10000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="135000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -200,43 +235,43 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="75000"/>
-                <a:satMod val="160000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="62000">
-              <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="125000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="140000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="12700">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -246,123 +281,91 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="50800" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="43137"/>
+                <a:alpha val="38000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="50800" dist="38100" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="61176"/>
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
           <a:scene3d>
-            <a:camera prst="orthographicFront" fov="0">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="contrasting" dir="t">
-              <a:rot lat="0" lon="0" rev="16500000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d contourW="12700" prstMaterial="powder">
-            <a:bevelT h="50800"/>
-            <a:contourClr>
-              <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="100000"/>
-              </a:schemeClr>
-            </a:contourClr>
-          </a:sp3d>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:reflection blurRad="12700" stA="25000" endPos="28000" dist="38100" dir="5400000" sy="-100000" rotWithShape="0"/>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront" fov="0">
+            <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
             <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="139700" h="38100"/>
-            <a:contourClr>
-              <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="100000"/>
-              </a:schemeClr>
-            </a:contourClr>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="100000"/>
-            <a:shade val="100000"/>
-            <a:satMod val="100000"/>
-          </a:schemeClr>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="50000"/>
-                <a:satMod val="145000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="70000"/>
-                <a:satMod val="145000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="85000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="155000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="50000"/>
-                <a:satMod val="145000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="30000">
-              <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="65000"/>
-                <a:satMod val="155000"/>
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="60000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="170000"/>
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -373,19 +376,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.microsoft.com/office/excel/2006/2" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:2" customFormat="1">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -393,7 +391,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:2" customFormat="1">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -401,7 +399,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="3" spans="1:2" customFormat="1">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -409,7 +407,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="4" spans="1:2" customFormat="1">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -417,7 +415,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="5" spans="1:2" customFormat="1">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -425,7 +423,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="6" spans="1:2" customFormat="1">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -433,7 +431,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="7" spans="1:2" customFormat="1">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -441,7 +439,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="8" spans="1:2" customFormat="1">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -449,7 +447,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="9" spans="1:2" customFormat="1">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -457,7 +455,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="10" spans="1:2" customFormat="1">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -467,43 +465,33 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection objects="0" scenarios="0"/>
-  <printOptions/>
-  <pageMargins left="0.35" right="0.35" top="0.75" bottom="0.75" header="0.25" footer="0.25"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.microsoft.com/office/excel/2006/2" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
-  <sheetProtection objects="0" scenarios="0"/>
-  <printOptions/>
-  <pageMargins left="0.35" right="0.35" top="0.75" bottom="0.75" header="0.25" footer="0.25"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.microsoft.com/office/excel/2006/2" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
-  <sheetProtection objects="0" scenarios="0"/>
-  <printOptions/>
-  <pageMargins left="0.35" right="0.35" top="0.75" bottom="0.75" header="0.25" footer="0.25"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Preserve rich text across read-write of SharedStringsTable, also improved performance and removed obsolete ole2-specific stuff
git-svn-id: https://svn.apache.org/repos/asf/poi/branches/ooxml@695832 13f79535-47bb-0310-9956-ffa450edef68
</commit_message>
<xml_diff>
--- a/src/testcases/org/apache/poi/hssf/data/sample.xlsx
+++ b/src/testcases/org/apache/poi/hssf/data/sample.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="20055" windowHeight="12240"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="19320" windowHeight="12120"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="rich test" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>Lorem</t>
   </si>
@@ -46,18 +46,293 @@
   </si>
   <si>
     <t>at</t>
+  </si>
+  <si>
+    <t>hello, xssf</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>hello</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, xssf</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">hello, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>xssf</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>hello</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, xssf</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>quick</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>brown</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> fox </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="14"/>
+        <color theme="9" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>jumps</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>over the lazy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="3" tint="0.39997558519241921"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dog</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Courier"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="14"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -81,8 +356,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,12 +749,52 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18.75">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>